<commit_message>
Timeout added to updated library activity in workflow. Config changed to low supervision. Final push before BAU?
</commit_message>
<xml_diff>
--- a/Documents/Config/config_Win7.xlsx
+++ b/Documents/Config/config_Win7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B5DBC3-638C-4FD3-80EC-33E8A97A396D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF5200A-8FDE-4B1A-8CFD-E32D977B6C3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12435" yWindow="1515" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="45" windowWidth="14400" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,7 +1114,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>79</v>
@@ -1125,7 +1125,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>80</v>
@@ -1136,7 +1136,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>81</v>
@@ -1147,7 +1147,7 @@
         <v>75</v>
       </c>
       <c r="B8" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>82</v>
@@ -1158,7 +1158,7 @@
         <v>76</v>
       </c>
       <c r="B9" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>83</v>
@@ -1169,7 +1169,7 @@
         <v>77</v>
       </c>
       <c r="B10" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>84</v>
@@ -1180,7 +1180,7 @@
         <v>78</v>
       </c>
       <c r="B11" s="7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>85</v>

</xml_diff>